<commit_message>
Use a few more fonts in the font names example, and sort them.
</commit_message>
<xml_diff>
--- a/src/Tests/RegressionTests/Expected/FontNameSize.xlsx
+++ b/src/Tests/RegressionTests/Expected/FontNameSize.xlsx
@@ -22,28 +22,58 @@
     <x:t>Algerian</x:t>
   </x:si>
   <x:si>
-    <x:t>Book Antiqua</x:t>
-  </x:si>
-  <x:si>
     <x:t>Arial</x:t>
   </x:si>
   <x:si>
+    <x:t>Arial Black</x:t>
+  </x:si>
+  <x:si>
     <x:t>Arial Narrow</x:t>
   </x:si>
   <x:si>
-    <x:t>Arial Black</x:t>
-  </x:si>
-  <x:si>
     <x:t>Arial Rounded MT Bold</x:t>
   </x:si>
   <x:si>
     <x:t>Bahnschrift</x:t>
   </x:si>
   <x:si>
+    <x:t>Barlow Condensed</x:t>
+  </x:si>
+  <x:si>
     <x:t>Barlow Condensed Black</x:t>
   </x:si>
   <x:si>
-    <x:t>Barlow Condensed</x:t>
+    <x:t>Barlow Condensed ExtraBold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barlow Condensed ExtraLight</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barlow Condensed Light</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barlow Condensed Medium</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barlow Condensed SemiBold</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Barlow Condensed Thin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baskerville Old Face</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bauhaus 93</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bell MT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Berlin Sans FB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Berlin Sans FB Demi</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -53,7 +83,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="11">
+  <x:fonts count="21">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -79,14 +109,14 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="14"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Book Antiqua"/>
+      <x:name val="Arial"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="16"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Arial"/>
+      <x:name val="Arial Black"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
@@ -100,21 +130,21 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="20"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Arial Black"/>
+      <x:name val="Arial Rounded MT Bold"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="22"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Arial Rounded MT Bold"/>
+      <x:name val="Bahnschrift"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="24"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Bahnschrift"/>
+      <x:name val="Barlow Condensed"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
@@ -128,7 +158,77 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="28"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Barlow Condensed"/>
+      <x:name val="Barlow Condensed ExtraBold"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="30"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Barlow Condensed ExtraLight"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="32"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Barlow Condensed Light"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="34"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Barlow Condensed Medium"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="36"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Barlow Condensed SemiBold"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="38"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Barlow Condensed Thin"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="40"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Baskerville Old Face"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="42"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Bauhaus 93"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="44"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Bell MT"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="46"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Berlin Sans FB"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="48"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Berlin Sans FB Demi"/>
       <x:family val="2"/>
     </x:font>
   </x:fonts>
@@ -159,7 +259,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -193,8 +293,38 @@
     <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -236,6 +366,46 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -534,7 +704,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A10"/>
+  <x:dimension ref="A1:A20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -590,6 +760,56 @@
         <x:v>9</x:v>
       </x:c>
     </x:row>
+    <x:row r="11" spans="1:1">
+      <x:c r="A11" s="11" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:1">
+      <x:c r="A12" s="12" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:1">
+      <x:c r="A13" s="13" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:1">
+      <x:c r="A14" s="14" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:1">
+      <x:c r="A15" s="15" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:1">
+      <x:c r="A16" s="16" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:1">
+      <x:c r="A17" s="17" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:1">
+      <x:c r="A18" s="18" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:1">
+      <x:c r="A19" s="19" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:1">
+      <x:c r="A20" s="20" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>